<commit_message>
Remove timescales from proportion parameters
</commit_message>
<xml_diff>
--- a/atomica/library/malaria_framework.xlsx
+++ b/atomica/library/malaria_framework.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\atomica\atomica\library\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\romesh\projects\atomica\atomica\library\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A31E0FBD-E4AE-42F8-9A76-5B3110476765}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26C5E764-B8EB-46E7-9B8C-1BF9CB69EA88}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="5055" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2430" yWindow="4935" windowWidth="29895" windowHeight="12645" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="9" r:id="rId1"/>
@@ -4867,7 +4867,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
@@ -7138,11 +7138,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:R182"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D43" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="D80" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F50" sqref="F50"/>
+      <selection pane="bottomRight" activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8134,9 +8134,6 @@
       <c r="C27" s="43" t="s">
         <v>33</v>
       </c>
-      <c r="D27" s="46">
-        <v>1</v>
-      </c>
       <c r="E27" s="43">
         <v>0</v>
       </c>
@@ -8530,9 +8527,6 @@
       </c>
       <c r="C35" s="43" t="s">
         <v>33</v>
-      </c>
-      <c r="D35" s="46">
-        <v>1</v>
       </c>
       <c r="E35" s="43">
         <v>0</v>
@@ -13845,7 +13839,7 @@
       <formula>NOT(ISERROR(SEARCH("y",J164)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="2">
+  <dataValidations disablePrompts="1" count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K131:M134 K16:M16 K84:M129 K11:M13 K18:M18 K20:M22 K69:M82 K24:M25 K27:M66" xr:uid="{00000000-0002-0000-0500-000000000000}">
       <formula1>"y,n"</formula1>
     </dataValidation>

</xml_diff>